<commit_message>
Temp save working version
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Desktop\WebScraping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\PycharmProjects\WebScraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD70E7F-FCA3-416E-BC69-809F28AEF18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3355BCFF-2BEE-4D7A-A41E-F292E63ABB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -20,47 +20,77 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t xml:space="preserve">Email </t>
-  </si>
-  <si>
-    <t>ZipCode</t>
-  </si>
-  <si>
-    <t>Google Url</t>
-  </si>
-  <si>
-    <t>163-8080</t>
-  </si>
-  <si>
-    <t>164-0011</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>141-0022</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>105-0001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dest1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dest2</t>
-  </si>
-  <si>
-    <t>Dest3</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>銀座駅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>十条駅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>東京都新宿区北新宿2-19-2-302</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>恵比寿駅</t>
+  </si>
+  <si>
+    <t>Origin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中目黒駅</t>
+  </si>
+  <si>
+    <t>渋谷駅</t>
+  </si>
+  <si>
+    <t>麻布十番駅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新宿駅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日本橋駅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>代官山駅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>六本木駅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beemars</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>早稲田大学3号館</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>飯田橋駅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大手町駅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Harry's Sandwich</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -75,6 +105,19 @@
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
     </font>
   </fonts>
   <fills count="2">
@@ -99,13 +142,19 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -121,7 +170,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -417,52 +466,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B5" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20240720 Update - Scrape duration Overall update to the code so it is usable again and improved the README.md
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\PycharmProjects\WebScraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3355BCFF-2BEE-4D7A-A41E-F292E63ABB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF626F12-C7AB-4E32-BBFC-E7105FF75893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,21 +26,9 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>十条駅</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>東京都新宿区北新宿2-19-2-302</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>恵比寿駅</t>
   </si>
   <si>
-    <t>Origin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>中目黒駅</t>
   </si>
   <si>
@@ -67,14 +55,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Beemars</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>早稲田大学3号館</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>飯田橋駅</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -83,7 +63,28 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Harry's Sandwich</t>
+    <t>Origin - Destination</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>浅草寺</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上野駅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>豊洲駅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>東京タワー</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>東京スカイツリー</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -466,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -480,50 +481,16 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="G1" s="2"/>
+      <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
@@ -532,7 +499,67 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>